<commit_message>
Started filling in benchmarks to get Dimitar started.
</commit_message>
<xml_diff>
--- a/PLDI-2012/Performance_Evaluation.xlsx
+++ b/PLDI-2012/Performance_Evaluation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Benchmark Name</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>9-Grades.xls (modified)</t>
+  </si>
+  <si>
+    <t>TRAIL%20INVENTORY%20N#A850A.XLS</t>
+  </si>
+  <si>
+    <t>2002fairreport.xls</t>
+  </si>
+  <si>
+    <t>104r.xls</t>
+  </si>
+  <si>
+    <t>Inventory_Control.xls</t>
   </si>
 </sst>
 </file>
@@ -372,15 +384,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
@@ -407,6 +419,26 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>